<commit_message>
looking for periodicity in calibration data
</commit_message>
<xml_diff>
--- a/testout.xlsx
+++ b/testout.xlsx
@@ -404,7 +404,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -485,34 +485,34 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>976.9958268700276</v>
+        <v>1197.857903352064</v>
       </c>
       <c r="C3">
-        <v>0.06693323423986935</v>
+        <v>0.02418958404227375</v>
       </c>
       <c r="D3">
-        <v>5269.977296650034</v>
+        <v>4839.230347984118</v>
       </c>
       <c r="E3">
-        <v>50.62849933600509</v>
+        <v>145.8281156512236</v>
       </c>
       <c r="F3">
-        <v>11.02045835189732</v>
+        <v>4.993146533125671</v>
       </c>
       <c r="G3">
-        <v>0.2864262315924695</v>
+        <v>0.04975375404840317</v>
       </c>
       <c r="H3">
-        <v>0.5540580043595069</v>
+        <v>2.120412158627037</v>
       </c>
       <c r="I3">
-        <v>0.5442602015057524</v>
+        <v>0.02112865401262505</v>
       </c>
       <c r="J3">
-        <v>5.427333401477833</v>
+        <v>0</v>
       </c>
       <c r="K3">
-        <v>0.1998097304273172</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -520,174 +520,171 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>984.7608490935352</v>
+        <v>1203.957903352064</v>
       </c>
       <c r="C4">
-        <v>0.1116730246550517</v>
+        <v>0.02418958402560949</v>
       </c>
       <c r="D4">
-        <v>1749.311345750166</v>
+        <v>22182.08512892421</v>
       </c>
       <c r="E4">
-        <v>145.3728646052253</v>
+        <v>203.8850007342618</v>
       </c>
       <c r="F4">
-        <v>5.368518105944267</v>
+        <v>4.993146533125671</v>
       </c>
       <c r="G4">
-        <v>0.7560903510205583</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>0.5540580043595069</v>
+        <v>2.120412158627037</v>
       </c>
       <c r="I4">
-        <v>0.5442602013202411</v>
+        <v>0.021128653986307</v>
       </c>
       <c r="J4">
-        <v>2.514723193216889</v>
+        <v>0</v>
       </c>
       <c r="K4">
-        <v>0.4016978145675571</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B5">
-        <v>964.2757148036692</v>
+        <v>1203.504392591808</v>
       </c>
       <c r="C5">
-        <v>0.07763030193916028</v>
+        <v>36555203.20718185</v>
       </c>
       <c r="D5">
-        <v>2457.244386116776</v>
+        <v>12352.05882945671</v>
       </c>
       <c r="E5">
-        <v>134.9423570232219</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>6.615403478554695</v>
+        <v>4</v>
       </c>
       <c r="G5">
-        <v>0.5059613364383578</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>0.5540580043595069</v>
-      </c>
-      <c r="I5">
-        <v>0.5442602013202411</v>
+        <v>0.1295442332920966</v>
       </c>
       <c r="J5">
-        <v>3.169897726294316</v>
+        <v>0</v>
       </c>
       <c r="K5">
-        <v>0.2634538195724769</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B6">
-        <v>984.860781501072</v>
+        <v>1204.5</v>
       </c>
       <c r="C6">
-        <v>0.121336944653126</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>760.9600363608489</v>
+        <v>11702.99999996422</v>
       </c>
       <c r="E6">
-        <v>37.07759749490266</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>5.405369836743553</v>
+        <v>4</v>
       </c>
       <c r="G6">
-        <v>0.4924832350942978</v>
+        <v>0</v>
       </c>
       <c r="H6">
-        <v>0.387208900434491</v>
+        <v>0.1295442332920966</v>
       </c>
       <c r="I6">
-        <v>0.8287470051577419</v>
+        <v>0</v>
       </c>
       <c r="J6">
-        <v>2.620243793775816</v>
+        <v>0</v>
       </c>
       <c r="K6">
-        <v>0.4201573075923415</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7">
-        <v>964.3718349185516</v>
+        <v>1203.747021279334</v>
       </c>
       <c r="C7">
-        <v>0.07694780567914587</v>
+        <v>6.092263274287248</v>
       </c>
       <c r="D7">
-        <v>1189.629983981775</v>
+        <v>2078.070078159463</v>
       </c>
       <c r="E7">
-        <v>64.51708644118392</v>
+        <v>17164.74093622674</v>
       </c>
       <c r="F7">
-        <v>6.926654417446674</v>
+        <v>5.513278424015677</v>
       </c>
       <c r="G7">
-        <v>0.5286905859793406</v>
+        <v>2.106331231357716</v>
       </c>
       <c r="H7">
-        <v>0.387208900434491</v>
+        <v>2.341293716621779</v>
       </c>
       <c r="I7">
-        <v>0.8287470071080756</v>
+        <v>0.894484133972382</v>
       </c>
       <c r="J7">
-        <v>3.398931422775887</v>
+        <v>0</v>
       </c>
       <c r="K7">
-        <v>0.2692452691470586</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8">
-        <v>976.9098525304828</v>
+        <v>1204.5</v>
       </c>
       <c r="C8">
-        <v>0.06942429944127118</v>
+        <v>6.092263290770176</v>
       </c>
       <c r="D8">
-        <v>2211.653362445873</v>
+        <v>0.0003458430366332567</v>
       </c>
       <c r="E8">
-        <v>62.65619282704587</v>
+        <v>16109.18909948876</v>
       </c>
       <c r="F8">
-        <v>10.71643306425441</v>
+        <v>5.513278424015677</v>
       </c>
       <c r="G8">
-        <v>0.4379039020642432</v>
+        <v>0</v>
       </c>
       <c r="H8">
-        <v>0.387208900434491</v>
+        <v>2.341293716621779</v>
       </c>
       <c r="I8">
-        <v>0.8287470071080756</v>
+        <v>0.8944841361765448</v>
       </c>
       <c r="J8">
-        <v>5.31655082136299</v>
+        <v>0</v>
       </c>
       <c r="K8">
-        <v>0.2206512294718354</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -695,34 +692,34 @@
         <v>1</v>
       </c>
       <c r="B9">
-        <v>977.0105391680647</v>
+        <v>1201.313659149814</v>
       </c>
       <c r="C9">
-        <v>0.1830363034961804</v>
+        <v>1.653173431720637</v>
       </c>
       <c r="D9">
-        <v>288.726526517694</v>
+        <v>705.4049387176522</v>
       </c>
       <c r="E9">
-        <v>10.76087020373514</v>
+        <v>1832.343690924262</v>
       </c>
       <c r="F9">
-        <v>10.55794916426737</v>
+        <v>5.45908566095081</v>
       </c>
       <c r="G9">
-        <v>0.7189716401154804</v>
+        <v>5.412096032064066</v>
       </c>
       <c r="H9">
-        <v>0.0001468034913862937</v>
+        <v>2.318279973093526</v>
       </c>
       <c r="I9">
-        <v>244.4624017045557</v>
+        <v>2.298325152493521</v>
       </c>
       <c r="J9">
-        <v>5.27895846927131</v>
+        <v>0</v>
       </c>
       <c r="K9">
-        <v>0.3594847220909395</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -730,174 +727,174 @@
         <v>2</v>
       </c>
       <c r="B10">
-        <v>964.2457248357463</v>
+        <v>1204.5</v>
       </c>
       <c r="C10">
-        <v>0.1262353184058511</v>
+        <v>1.65317343243369</v>
       </c>
       <c r="D10">
-        <v>198.5974435122717</v>
+        <v>2533.812261960868</v>
       </c>
       <c r="E10">
-        <v>9.465822320995162</v>
+        <v>2572.576680216918</v>
       </c>
       <c r="F10">
-        <v>5.942609403378138</v>
+        <v>5.45908566095081</v>
       </c>
       <c r="G10">
-        <v>0.5178948802643074</v>
+        <v>0</v>
       </c>
       <c r="H10">
-        <v>0.0001468034913862937</v>
+        <v>2.318279973093526</v>
       </c>
       <c r="I10">
-        <v>244.4624020417737</v>
+        <v>2.298325146166922</v>
       </c>
       <c r="J10">
-        <v>2.971295625081115</v>
+        <v>0</v>
       </c>
       <c r="K10">
-        <v>0.2589466505762839</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B11">
-        <v>984.7086813222916</v>
+        <v>1197.694094758245</v>
       </c>
       <c r="C11">
-        <v>0.3292667386743013</v>
+        <v>0.05069023981001947</v>
       </c>
       <c r="D11">
-        <v>90.54076949013329</v>
+        <v>512.0940041707535</v>
       </c>
       <c r="E11">
-        <v>12.2697570809066</v>
+        <v>38.46466755958183</v>
       </c>
       <c r="F11">
-        <v>5.641197983910077</v>
+        <v>4.785790835322817</v>
       </c>
       <c r="G11">
-        <v>1.438090052081606</v>
+        <v>0.1112517475686959</v>
       </c>
       <c r="H11">
-        <v>0.0001468034913862937</v>
+        <v>2.032355551462631</v>
       </c>
       <c r="I11">
-        <v>244.4624020417737</v>
+        <v>0.04724466964239888</v>
       </c>
       <c r="J11">
-        <v>2.820590374591045</v>
+        <v>0</v>
       </c>
       <c r="K11">
-        <v>0.7190428374134309</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B12">
-        <v>963.9721913491618</v>
+        <v>1203.794094758245</v>
       </c>
       <c r="C12">
-        <v>0.2266106949361216</v>
+        <v>0.0506902396846848</v>
       </c>
       <c r="D12">
-        <v>265.1319258124017</v>
+        <v>2293.061155800896</v>
       </c>
       <c r="E12">
-        <v>16.71211000131717</v>
+        <v>47.4478860606395</v>
       </c>
       <c r="F12">
-        <v>6.756836837933291</v>
+        <v>4.785790835322817</v>
       </c>
       <c r="G12">
-        <v>0.9363461673629077</v>
+        <v>0</v>
       </c>
       <c r="H12">
-        <v>0.001084616078520728</v>
+        <v>2.032355551462631</v>
       </c>
       <c r="I12">
-        <v>741.1893984076025</v>
+        <v>0.04724466953752718</v>
       </c>
       <c r="J12">
-        <v>3.378407592414364</v>
+        <v>0</v>
       </c>
       <c r="K12">
-        <v>0.761466879704819</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B13">
-        <v>976.9069884490056</v>
+        <v>1204.287022712923</v>
       </c>
       <c r="C13">
-        <v>0.2608295280841544</v>
+        <v>14721839.54820037</v>
       </c>
       <c r="D13">
-        <v>478.5370547031059</v>
+        <v>0.000145331255725825</v>
       </c>
       <c r="E13">
-        <v>35.03019109964486</v>
+        <v>4333.134871143917</v>
       </c>
       <c r="F13">
-        <v>11.83999637906345</v>
+        <v>7.818376439848815</v>
       </c>
       <c r="G13">
-        <v>1.230848004252382</v>
+        <v>1.687234718544879</v>
       </c>
       <c r="H13">
-        <v>0.001084616078520728</v>
+        <v>3.320187051150046</v>
       </c>
       <c r="I13">
-        <v>741.1893996466929</v>
+        <v>0.7165087177245144</v>
       </c>
       <c r="J13">
-        <v>5.919979830959162</v>
+        <v>0</v>
       </c>
       <c r="K13">
-        <v>0.6154221546327732</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B14">
-        <v>984.8183730372119</v>
+        <v>1204.5</v>
       </c>
       <c r="C14">
-        <v>0.385061087749774</v>
+        <v>14721839.58168015</v>
       </c>
       <c r="D14">
-        <v>153.1225575276227</v>
+        <v>886.0835445511739</v>
       </c>
       <c r="E14">
-        <v>38.97742044492804</v>
+        <v>3392.563418859803</v>
       </c>
       <c r="F14">
-        <v>5.196194099803753</v>
+        <v>7.818376439848815</v>
       </c>
       <c r="G14">
-        <v>2.676535809162644</v>
+        <v>0</v>
       </c>
       <c r="H14">
-        <v>0.001084616078520728</v>
+        <v>3.320187051150046</v>
       </c>
       <c r="I14">
-        <v>741.1893996466929</v>
+        <v>0.7165087168556591</v>
       </c>
       <c r="J14">
-        <v>2.598088448447049</v>
+        <v>0</v>
       </c>
       <c r="K14">
-        <v>1.338264169263061</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -905,34 +902,34 @@
         <v>1</v>
       </c>
       <c r="B15">
-        <v>964.256701458867</v>
+        <v>1197.670237009553</v>
       </c>
       <c r="C15">
-        <v>0.1191015774253873</v>
+        <v>0.0835099746552289</v>
       </c>
       <c r="D15">
-        <v>246.63450760156</v>
+        <v>308.5625065689817</v>
       </c>
       <c r="E15">
-        <v>7.804864315344095</v>
+        <v>36.27050021105089</v>
       </c>
       <c r="F15">
-        <v>6.731665300646332</v>
+        <v>5.096344126016659</v>
       </c>
       <c r="G15">
-        <v>0.465680017223186</v>
+        <v>0.1875844850396162</v>
       </c>
       <c r="H15">
-        <v>6.712633278382896E-05</v>
+        <v>2.16423651452274</v>
       </c>
       <c r="I15">
-        <v>78.16176432016206</v>
+        <v>0.07966047485239894</v>
       </c>
       <c r="J15">
-        <v>3.365822378771749</v>
+        <v>0</v>
       </c>
       <c r="K15">
-        <v>0.2301331672080193</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -940,279 +937,34 @@
         <v>2</v>
       </c>
       <c r="B16">
-        <v>984.9881603981223</v>
+        <v>1203.770237009553</v>
       </c>
       <c r="C16">
-        <v>0.1350229825866293</v>
+        <v>0.08350997449280832</v>
       </c>
       <c r="D16">
-        <v>191.5127941483226</v>
+        <v>1413.512358351985</v>
       </c>
       <c r="E16">
-        <v>11.22914492010974</v>
+        <v>45.74899937532195</v>
       </c>
       <c r="F16">
-        <v>5.262505640206327</v>
+        <v>5.096344126016659</v>
       </c>
       <c r="G16">
-        <v>0.6044666344638429</v>
+        <v>0</v>
       </c>
       <c r="H16">
-        <v>6.712633278382896E-05</v>
+        <v>2.16423651452274</v>
       </c>
       <c r="I16">
-        <v>78.16176439876075</v>
+        <v>0.07966047489795509</v>
       </c>
       <c r="J16">
-        <v>2.631244789285967</v>
+        <v>0</v>
       </c>
       <c r="K16">
-        <v>0.3022323959082456</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11">
-      <c r="A17">
-        <v>3</v>
-      </c>
-      <c r="B17">
-        <v>976.9821840176904</v>
-      </c>
-      <c r="C17">
-        <v>0.09946954040277992</v>
-      </c>
-      <c r="D17">
-        <v>487.8920708027577</v>
-      </c>
-      <c r="E17">
-        <v>6.468473786914505</v>
-      </c>
-      <c r="F17">
-        <v>10.40439801039621</v>
-      </c>
-      <c r="G17">
-        <v>0.4133165795364026</v>
-      </c>
-      <c r="H17">
-        <v>6.712633278382896E-05</v>
-      </c>
-      <c r="I17">
-        <v>78.16176439876075</v>
-      </c>
-      <c r="J17">
-        <v>5.20218313137731</v>
-      </c>
-      <c r="K17">
-        <v>0.2066576577220822</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11">
-      <c r="A18">
-        <v>1</v>
-      </c>
-      <c r="B18">
-        <v>964.6804049055567</v>
-      </c>
-      <c r="C18">
-        <v>0.3325891092716559</v>
-      </c>
-      <c r="D18">
-        <v>112.7586197399874</v>
-      </c>
-      <c r="E18">
-        <v>9.265257472921759</v>
-      </c>
-      <c r="F18">
-        <v>7.543871667045455</v>
-      </c>
-      <c r="G18">
-        <v>1.440949305321746</v>
-      </c>
-      <c r="H18">
-        <v>1.505688460736466</v>
-      </c>
-      <c r="I18">
-        <v>1.265621021748307</v>
-      </c>
-      <c r="J18">
-        <v>2.892035255397404</v>
-      </c>
-      <c r="K18">
-        <v>1.115592306684834</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
-      <c r="A19">
-        <v>2</v>
-      </c>
-      <c r="B19">
-        <v>976.8412613277346</v>
-      </c>
-      <c r="C19">
-        <v>0.2953146066591111</v>
-      </c>
-      <c r="D19">
-        <v>214.1415499581353</v>
-      </c>
-      <c r="E19">
-        <v>37.83927687888555</v>
-      </c>
-      <c r="F19">
-        <v>9.05388068797272</v>
-      </c>
-      <c r="G19">
-        <v>2.567225998640566</v>
-      </c>
-      <c r="H19">
-        <v>1.505688460736466</v>
-      </c>
-      <c r="I19">
-        <v>1.265621020020655</v>
-      </c>
-      <c r="J19">
-        <v>3.789990042073362</v>
-      </c>
-      <c r="K19">
-        <v>1.487629209465292</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11">
-      <c r="A20">
-        <v>3</v>
-      </c>
-      <c r="B20">
-        <v>985.0020222906896</v>
-      </c>
-      <c r="C20">
-        <v>0.7336348097735542</v>
-      </c>
-      <c r="D20">
-        <v>87.33745618616368</v>
-      </c>
-      <c r="E20">
-        <v>29.67943959046524</v>
-      </c>
-      <c r="F20">
-        <v>8.487586526572116</v>
-      </c>
-      <c r="G20">
-        <v>3.095843239285174</v>
-      </c>
-      <c r="H20">
-        <v>1.505688460736466</v>
-      </c>
-      <c r="I20">
-        <v>1.265621020020655</v>
-      </c>
-      <c r="J20">
-        <v>3.458951902992458</v>
-      </c>
-      <c r="K20">
-        <v>1.826522007297614</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11">
-      <c r="A21">
-        <v>1</v>
-      </c>
-      <c r="B21">
-        <v>976.9978153956583</v>
-      </c>
-      <c r="C21">
-        <v>0.2145063823346433</v>
-      </c>
-      <c r="D21">
-        <v>358.4918743223126</v>
-      </c>
-      <c r="E21">
-        <v>11.3092209250086</v>
-      </c>
-      <c r="F21">
-        <v>11.03676608966816</v>
-      </c>
-      <c r="G21">
-        <v>0.9312158749983186</v>
-      </c>
-      <c r="H21">
-        <v>0.001801773247576133</v>
-      </c>
-      <c r="I21">
-        <v>506.5619167328006</v>
-      </c>
-      <c r="J21">
-        <v>5.518365331440429</v>
-      </c>
-      <c r="K21">
-        <v>0.5994461659946007</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11">
-      <c r="A22">
-        <v>2</v>
-      </c>
-      <c r="B22">
-        <v>984.5455266618928</v>
-      </c>
-      <c r="C22">
-        <v>0.3898263586003557</v>
-      </c>
-      <c r="D22">
-        <v>107.6202365627789</v>
-      </c>
-      <c r="E22">
-        <v>30.62654368408154</v>
-      </c>
-      <c r="F22">
-        <v>5.149554495077666</v>
-      </c>
-      <c r="G22">
-        <v>2.709077959130235</v>
-      </c>
-      <c r="H22">
-        <v>0.001801773247576133</v>
-      </c>
-      <c r="I22">
-        <v>506.5619176723274</v>
-      </c>
-      <c r="J22">
-        <v>2.574767513785409</v>
-      </c>
-      <c r="K22">
-        <v>1.354535835367524</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11">
-      <c r="A23">
-        <v>3</v>
-      </c>
-      <c r="B23">
-        <v>964.2752753021214</v>
-      </c>
-      <c r="C23">
-        <v>0.2694597737766926</v>
-      </c>
-      <c r="D23">
-        <v>156.5603680940074</v>
-      </c>
-      <c r="E23">
-        <v>27.68474029558721</v>
-      </c>
-      <c r="F23">
-        <v>6.571879799732613</v>
-      </c>
-      <c r="G23">
-        <v>1.718165542861244</v>
-      </c>
-      <c r="H23">
-        <v>0.001801773247576133</v>
-      </c>
-      <c r="I23">
-        <v>506.5619176723274</v>
-      </c>
-      <c r="J23">
-        <v>3.285928402675342</v>
-      </c>
-      <c r="K23">
-        <v>0.8590805363707241</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>